<commit_message>
Updates to reference data and mappings for CVS drugs
</commit_message>
<xml_diff>
--- a/vignettes/web/issues-2022-12-07.xlsx
+++ b/vignettes/web/issues-2022-12-07.xlsx
@@ -1,70 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Items by number of issues" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Missing items by field" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Inconsistent entries" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Data quality list" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Items by number of issues" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing items by field" sheetId="2" r:id="rId2"/>
+    <sheet name="Inconsistent entries" sheetId="3" r:id="rId3"/>
+    <sheet name="Data quality list" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">issues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Items with issues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient subgroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.row_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.error_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.subgroup</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,61 +55,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="issues"/>
-    <tableColumn id="2" name="item count"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="patient subgroup"/>
-    <tableColumn id="2" name="missing value"/>
-    <tableColumn id="3" name="n"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:B2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B2"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="error"/>
-    <tableColumn id="2" name="n"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name=".row_number"/>
-    <tableColumn id="2" name=".error_type"/>
-    <tableColumn id="3" name=".variable"/>
-    <tableColumn id="4" name=".subgroup"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -193,6 +115,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -218,12 +144,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -249,7 +178,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,178 +353,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="10.71" hidden="0" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>issues</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>item count</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total items</t>
+        </is>
+      </c>
+      <c r="B2">
         <v>18009</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Items with issues</t>
+        </is>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="3.71" hidden="0" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>patient subgroup</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>missing value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId4"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="5.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="3.71" hidden="0" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId5"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="9.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>.row_number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>.error_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>.variable</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>.subgroup</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId6"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>